<commit_message>
could be a final commit
</commit_message>
<xml_diff>
--- a/RefineCalc/bin/Debug/RefineData.xlsx
+++ b/RefineCalc/bin/Debug/RefineData.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23901"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24931"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\NewFace\Desktop\RefineCalc\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\RefineCalc\RefineCalc\bin\Debug\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E73F60ED-04C7-4B05-8119-04940F522F35}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{458BD4FE-FA98-4779-BB7A-ECE0232B61E7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{1EF8837A-CC51-47D0-A690-844D2EFA9766}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{1EF8837A-CC51-47D0-A690-844D2EFA9766}"/>
   </bookViews>
   <sheets>
     <sheet name="무기" sheetId="1" r:id="rId1"/>
@@ -491,8 +491,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CB6FD220-EAE5-41A5-BBF8-61C46BFD0D2A}">
   <dimension ref="A1:N58"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K15" sqref="K15"/>
+    <sheetView topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="G34" sqref="G34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -564,7 +564,7 @@
         <v>60</v>
       </c>
       <c r="G2">
-        <v>400</v>
+        <v>120</v>
       </c>
       <c r="H2">
         <v>60</v>
@@ -608,7 +608,7 @@
         <v>60</v>
       </c>
       <c r="G3">
-        <v>400</v>
+        <v>120</v>
       </c>
       <c r="H3">
         <v>45</v>
@@ -652,7 +652,7 @@
         <v>60</v>
       </c>
       <c r="G4">
-        <v>400</v>
+        <v>120</v>
       </c>
       <c r="H4">
         <v>30</v>
@@ -696,7 +696,7 @@
         <v>74</v>
       </c>
       <c r="G5">
-        <v>400</v>
+        <v>120</v>
       </c>
       <c r="H5">
         <v>30</v>
@@ -740,7 +740,7 @@
         <v>74</v>
       </c>
       <c r="G6">
-        <v>400</v>
+        <v>120</v>
       </c>
       <c r="H6">
         <v>30</v>
@@ -784,7 +784,7 @@
         <v>74</v>
       </c>
       <c r="G7">
-        <v>400</v>
+        <v>120</v>
       </c>
       <c r="H7">
         <v>15</v>
@@ -828,7 +828,7 @@
         <v>88</v>
       </c>
       <c r="G8">
-        <v>400</v>
+        <v>120</v>
       </c>
       <c r="H8">
         <v>15</v>
@@ -872,7 +872,7 @@
         <v>88</v>
       </c>
       <c r="G9">
-        <v>400</v>
+        <v>120</v>
       </c>
       <c r="H9">
         <v>15</v>
@@ -916,7 +916,7 @@
         <v>88</v>
       </c>
       <c r="G10">
-        <v>400</v>
+        <v>120</v>
       </c>
       <c r="H10">
         <v>10</v>
@@ -960,7 +960,7 @@
         <v>120</v>
       </c>
       <c r="G11">
-        <v>400</v>
+        <v>120</v>
       </c>
       <c r="H11">
         <v>10</v>
@@ -1004,7 +1004,7 @@
         <v>164</v>
       </c>
       <c r="G12">
-        <v>400</v>
+        <v>120</v>
       </c>
       <c r="H12">
         <v>10</v>
@@ -1048,7 +1048,7 @@
         <v>222</v>
       </c>
       <c r="G13">
-        <v>400</v>
+        <v>120</v>
       </c>
       <c r="H13">
         <v>5</v>
@@ -1092,7 +1092,7 @@
         <v>300</v>
       </c>
       <c r="G14">
-        <v>400</v>
+        <v>120</v>
       </c>
       <c r="H14">
         <v>5</v>
@@ -1136,7 +1136,7 @@
         <v>406</v>
       </c>
       <c r="G15">
-        <v>400</v>
+        <v>120</v>
       </c>
       <c r="H15">
         <v>3</v>
@@ -1400,7 +1400,7 @@
         <v>156</v>
       </c>
       <c r="G21">
-        <v>640</v>
+        <v>320</v>
       </c>
       <c r="H21">
         <v>60</v>
@@ -1444,7 +1444,7 @@
         <v>156</v>
       </c>
       <c r="G22">
-        <v>640</v>
+        <v>320</v>
       </c>
       <c r="H22">
         <v>45</v>
@@ -1488,7 +1488,7 @@
         <v>156</v>
       </c>
       <c r="G23">
-        <v>640</v>
+        <v>320</v>
       </c>
       <c r="H23">
         <v>30</v>
@@ -1532,7 +1532,7 @@
         <v>192</v>
       </c>
       <c r="G24">
-        <v>640</v>
+        <v>320</v>
       </c>
       <c r="H24">
         <v>30</v>
@@ -1576,7 +1576,7 @@
         <v>192</v>
       </c>
       <c r="G25">
-        <v>660</v>
+        <v>330</v>
       </c>
       <c r="H25">
         <v>30</v>
@@ -1620,7 +1620,7 @@
         <v>192</v>
       </c>
       <c r="G26">
-        <v>660</v>
+        <v>330</v>
       </c>
       <c r="H26">
         <v>15</v>
@@ -1664,7 +1664,7 @@
         <v>228</v>
       </c>
       <c r="G27">
-        <v>660</v>
+        <v>330</v>
       </c>
       <c r="H27">
         <v>15</v>
@@ -1708,7 +1708,7 @@
         <v>228</v>
       </c>
       <c r="G28">
-        <v>660</v>
+        <v>330</v>
       </c>
       <c r="H28">
         <v>15</v>
@@ -1752,7 +1752,7 @@
         <v>228</v>
       </c>
       <c r="G29">
-        <v>660</v>
+        <v>330</v>
       </c>
       <c r="H29">
         <v>10</v>
@@ -1796,7 +1796,7 @@
         <v>310</v>
       </c>
       <c r="G30">
-        <v>680</v>
+        <v>410</v>
       </c>
       <c r="H30">
         <v>10</v>
@@ -1840,7 +1840,7 @@
         <v>422</v>
       </c>
       <c r="G31">
-        <v>680</v>
+        <v>480</v>
       </c>
       <c r="H31">
         <v>10</v>
@@ -1884,7 +1884,7 @@
         <v>572</v>
       </c>
       <c r="G32">
-        <v>680</v>
+        <v>540</v>
       </c>
       <c r="H32">
         <v>5</v>
@@ -1928,7 +1928,7 @@
         <v>776</v>
       </c>
       <c r="G33">
-        <v>710</v>
+        <v>640</v>
       </c>
       <c r="H33">
         <v>5</v>
@@ -2284,8 +2284,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{78C84CAA-97BA-4F22-877D-D8E4725A79A4}">
   <dimension ref="A1:N58"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="L1" sqref="L1:N1048576"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="G34" sqref="G34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -2354,7 +2354,7 @@
         <v>42</v>
       </c>
       <c r="G2">
-        <v>220</v>
+        <v>70</v>
       </c>
       <c r="H2">
         <v>60</v>
@@ -2398,7 +2398,7 @@
         <v>42</v>
       </c>
       <c r="G3">
-        <v>220</v>
+        <v>70</v>
       </c>
       <c r="H3">
         <v>45</v>
@@ -2442,7 +2442,7 @@
         <v>42</v>
       </c>
       <c r="G4">
-        <v>220</v>
+        <v>70</v>
       </c>
       <c r="H4">
         <v>30</v>
@@ -2486,7 +2486,7 @@
         <v>50</v>
       </c>
       <c r="G5">
-        <v>220</v>
+        <v>70</v>
       </c>
       <c r="H5">
         <v>30</v>
@@ -2530,7 +2530,7 @@
         <v>50</v>
       </c>
       <c r="G6">
-        <v>220</v>
+        <v>70</v>
       </c>
       <c r="H6">
         <v>30</v>
@@ -2574,7 +2574,7 @@
         <v>50</v>
       </c>
       <c r="G7">
-        <v>220</v>
+        <v>70</v>
       </c>
       <c r="H7">
         <v>15</v>
@@ -2618,7 +2618,7 @@
         <v>60</v>
       </c>
       <c r="G8">
-        <v>220</v>
+        <v>70</v>
       </c>
       <c r="H8">
         <v>15</v>
@@ -2662,7 +2662,7 @@
         <v>60</v>
       </c>
       <c r="G9">
-        <v>220</v>
+        <v>70</v>
       </c>
       <c r="H9">
         <v>15</v>
@@ -2706,7 +2706,7 @@
         <v>60</v>
       </c>
       <c r="G10">
-        <v>220</v>
+        <v>70</v>
       </c>
       <c r="H10">
         <v>10</v>
@@ -3190,7 +3190,7 @@
         <v>108</v>
       </c>
       <c r="G21">
-        <v>330</v>
+        <v>170</v>
       </c>
       <c r="H21">
         <v>60</v>
@@ -3234,7 +3234,7 @@
         <v>108</v>
       </c>
       <c r="G22">
-        <v>330</v>
+        <v>170</v>
       </c>
       <c r="H22">
         <v>45</v>
@@ -3278,7 +3278,7 @@
         <v>108</v>
       </c>
       <c r="G23">
-        <v>330</v>
+        <v>170</v>
       </c>
       <c r="H23">
         <v>30</v>
@@ -3322,7 +3322,7 @@
         <v>132</v>
       </c>
       <c r="G24">
-        <v>330</v>
+        <v>170</v>
       </c>
       <c r="H24">
         <v>30</v>
@@ -3366,7 +3366,7 @@
         <v>132</v>
       </c>
       <c r="G25">
-        <v>330</v>
+        <v>170</v>
       </c>
       <c r="H25">
         <v>30</v>
@@ -3410,7 +3410,7 @@
         <v>132</v>
       </c>
       <c r="G26">
-        <v>330</v>
+        <v>170</v>
       </c>
       <c r="H26">
         <v>15</v>
@@ -3454,7 +3454,7 @@
         <v>158</v>
       </c>
       <c r="G27">
-        <v>330</v>
+        <v>170</v>
       </c>
       <c r="H27">
         <v>15</v>
@@ -3498,7 +3498,7 @@
         <v>158</v>
       </c>
       <c r="G28">
-        <v>330</v>
+        <v>170</v>
       </c>
       <c r="H28">
         <v>15</v>
@@ -3542,7 +3542,7 @@
         <v>158</v>
       </c>
       <c r="G29">
-        <v>350</v>
+        <v>180</v>
       </c>
       <c r="H29">
         <v>10</v>
@@ -3586,7 +3586,7 @@
         <v>216</v>
       </c>
       <c r="G30">
-        <v>350</v>
+        <v>210</v>
       </c>
       <c r="H30">
         <v>10</v>
@@ -3630,7 +3630,7 @@
         <v>292</v>
       </c>
       <c r="G31">
-        <v>350</v>
+        <v>250</v>
       </c>
       <c r="H31">
         <v>10</v>
@@ -3674,7 +3674,7 @@
         <v>396</v>
       </c>
       <c r="G32">
-        <v>350</v>
+        <v>280</v>
       </c>
       <c r="H32">
         <v>5</v>
@@ -3718,7 +3718,7 @@
         <v>536</v>
       </c>
       <c r="G33">
-        <v>350</v>
+        <v>320</v>
       </c>
       <c r="H33">
         <v>5</v>

</xml_diff>